<commit_message>
BOM v0.0 is obsolete
BOM v0.1 is valid. Only a comment about a resistor is inserted, material is the same like v0.0
</commit_message>
<xml_diff>
--- a/Diag586220_Harness/Diag586220_User_Port/Rev.0/excel/Diag586220_UserPort_BOM_v0_0.xlsx
+++ b/Diag586220_Harness/Diag586220_User_Port/Rev.0/excel/Diag586220_UserPort_BOM_v0_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\Diag586220_Harness\Diag586220_User_Port\Rev.0\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\C64-Projects\Diag586220_Harness\Diag586220_User_Port\Rev.0\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC32EE3-1487-4274-9549-F12901F9626D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8939FF0-9DEB-4A68-96DA-C1DEE1D4CF74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2904" yWindow="2184" windowWidth="26448" windowHeight="13548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3264" yWindow="1464" windowWidth="26448" windowHeight="11904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -772,14 +772,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1280,7 +1280,7 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1294,24 +1294,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1508,7 +1508,7 @@
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -1517,7 +1517,7 @@
       <c r="E12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1580,7 +1580,7 @@
       <c r="E15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1611,14 +1611,14 @@
       <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1630,14 +1630,14 @@
       <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1649,14 +1649,14 @@
       <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1668,14 +1668,14 @@
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1684,17 +1684,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>67</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2200,6 +2200,7 @@
   <pageMargins left="0.70866141732283472" right="0.79166666666666663" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"Futura Lt BT,Light"&amp;F
 Drafted by Sven Petersen&amp;C&amp;"Futura Lt BT,Light"Page &amp;P of &amp;N&amp;R&amp;"Futura Lt BT,Light"&amp;D &amp;T
 Doc.No.: 113-5-01-00.0</oddFooter>
@@ -2207,8 +2208,9 @@
   <ignoredErrors>
     <ignoredError sqref="A4" calculatedColumn="1"/>
   </ignoredErrors>
+  <legacyDrawingHF r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>